<commit_message>
Compare Plan Test Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFile/ExcelData.xlsx
+++ b/src/test/resources/ExcelFile/ExcelData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
   <si>
     <t>TC</t>
   </si>
@@ -86,7 +86,16 @@
     <t>VerifyComparePlanMenuLauncherTest</t>
   </si>
   <si>
+    <t>ComparePlanCloseDrawerTest</t>
+  </si>
+  <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>CloseComparePlanTest</t>
+  </si>
+  <si>
+    <t>ContinueComparePlanTest</t>
   </si>
   <si>
     <t>OnePlus</t>
@@ -1370,10 +1379,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1533,7 +1542,49 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1610,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1568,12 +1619,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6">
         <v>12</v>
@@ -1581,7 +1632,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7"/>
     </row>
@@ -1590,12 +1641,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6">
         <v>13</v>
@@ -1623,16 +1674,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1663,24 +1714,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1709,19 +1760,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1729,16 +1780,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1746,16 +1797,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1763,16 +1814,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate Quote Scenarios test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFile/ExcelData.xlsx
+++ b/src/test/resources/ExcelFile/ExcelData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>TC</t>
   </si>
@@ -80,7 +80,7 @@
     <t>VerifyPolicyLoginMenuLauncherTest</t>
   </si>
   <si>
-    <t>GeneratingAQuoteForALeadTest</t>
+    <t>VerifyGenerateQuoteBackButtonTest</t>
   </si>
   <si>
     <t>VerifyComparePlanMenuLauncherTest</t>
@@ -89,13 +89,28 @@
     <t>ComparePlanCloseDrawerTest</t>
   </si>
   <si>
+    <t>CloseComparePlanTest</t>
+  </si>
+  <si>
+    <t>ContinueComparePlanTest</t>
+  </si>
+  <si>
+    <t>GenerateQuoteSearchFunctionalityTest</t>
+  </si>
+  <si>
+    <t>SelectingALeadFromGenerateQuotePageTest</t>
+  </si>
+  <si>
+    <t>GenerateQuoteCloseValidationTest</t>
+  </si>
+  <si>
+    <t>GenerateQuoteContinueButtonCloseValidationTest</t>
+  </si>
+  <si>
+    <t>GenerateQuoteExitButtonValidationTest</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>CloseComparePlanTest</t>
-  </si>
-  <si>
-    <t>ContinueComparePlanTest</t>
   </si>
   <si>
     <t>OnePlus</t>
@@ -1379,10 +1394,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1556,12 +1571,12 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -1570,12 +1585,12 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1584,7 +1599,77 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1695,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1619,12 +1704,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6">
         <v>12</v>
@@ -1632,7 +1717,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7"/>
     </row>
@@ -1641,12 +1726,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6">
         <v>13</v>
@@ -1674,16 +1759,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1714,24 +1799,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1760,19 +1845,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1780,16 +1865,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1797,16 +1882,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1814,16 +1899,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate Quote and Compare Plan Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFile/ExcelData.xlsx
+++ b/src/test/resources/ExcelFile/ExcelData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>TC</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>GenerateQuoteExitButtonValidationTest</t>
+  </si>
+  <si>
+    <t>VerifyComparePlanQuickLinkTest</t>
+  </si>
+  <si>
+    <t>GeneratingAQuoteForALeadTest</t>
   </si>
   <si>
     <t>Y</t>
@@ -1394,10 +1400,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1669,7 +1675,35 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1695,7 +1729,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1704,12 +1738,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6">
         <v>12</v>
@@ -1717,7 +1751,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7"/>
     </row>
@@ -1726,12 +1760,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6">
         <v>13</v>
@@ -1759,16 +1793,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1799,24 +1833,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1845,19 +1879,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1865,16 +1899,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1882,16 +1916,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1899,16 +1933,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>